<commit_message>
change table OrdersDetail in DB, Binding username, edit DetailOrder and addNewOrder Screen
Description set username at screens, edit and binding data at DetailOrderScreen, change DB - add 2 cols odDiscountedPrice & odTempPrice to Table: OrdersDetail
</commit_message>
<xml_diff>
--- a/Secondary data/ImportData-v1.xlsx
+++ b/Secondary data/ImportData-v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sources\GitHub\Project1_BookStore\Secondary data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5335492E-BC5B-4D99-94BA-802619FB6EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E797F6-1A70-48A1-A185-D2F26B1572D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9072" xr2:uid="{50692952-7C83-42D7-A757-ED8179832E1C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{50692952-7C83-42D7-A757-ED8179832E1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -385,31 +385,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -728,793 +722,764 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="4"/>
-    <col min="2" max="2" width="67.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.88671875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="20" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="11.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="67.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20" style="2" customWidth="1"/>
+    <col min="8" max="8" width="21" style="5" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="5"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="8" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="2:12" s="3" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="B1" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="6"/>
-    </row>
-    <row r="2" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" spans="2:12" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="3">
+      <c r="F2" s="2">
         <v>120000</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="2">
         <v>15</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="2">
         <v>2019</v>
       </c>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="2">
         <v>150000</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="2">
         <v>15</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="2">
         <v>2019</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="L3" s="5"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="L3" s="6"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="2">
         <v>188000</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G4" s="2">
         <v>10</v>
       </c>
-      <c r="G4" s="3">
+      <c r="H4" s="2">
         <v>2019</v>
       </c>
-      <c r="J4" s="1"/>
-      <c r="L4" s="5"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="L4" s="6"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="2">
         <v>159000</v>
       </c>
-      <c r="F5" s="3">
+      <c r="G5" s="2">
         <v>11</v>
       </c>
-      <c r="G5" s="3">
+      <c r="H5" s="2">
         <v>2021</v>
       </c>
-      <c r="J5" s="1"/>
-      <c r="L5" s="5"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="L5" s="6"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="3">
+      <c r="F6" s="2">
         <v>79000</v>
       </c>
-      <c r="F6" s="3">
+      <c r="G6" s="2">
         <v>17</v>
       </c>
-      <c r="G6" s="3">
+      <c r="H6" s="2">
         <v>2018</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="L6" s="5"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="L6" s="6"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="3">
+      <c r="F7" s="2">
         <v>139000</v>
       </c>
-      <c r="F7" s="3">
+      <c r="G7" s="2">
         <v>23</v>
       </c>
-      <c r="G7" s="3">
+      <c r="H7" s="2">
         <v>2018</v>
       </c>
-      <c r="J7" s="1"/>
-      <c r="L7" s="5"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="L7" s="6"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="3">
+      <c r="F8" s="2">
         <v>113000</v>
       </c>
-      <c r="F8" s="3">
+      <c r="G8" s="2">
         <v>13</v>
       </c>
-      <c r="G8" s="3">
+      <c r="H8" s="2">
         <v>2021</v>
       </c>
-      <c r="J8" s="1"/>
-      <c r="L8" s="5"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="L8" s="6"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="3">
+      <c r="F9" s="2">
         <v>109500</v>
       </c>
-      <c r="F9" s="3">
+      <c r="G9" s="2">
         <v>11</v>
       </c>
-      <c r="G9" s="3">
+      <c r="H9" s="2">
         <v>2018</v>
       </c>
-      <c r="J9" s="1"/>
-      <c r="L9" s="5"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="L9" s="6"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="3">
+      <c r="F10" s="2">
         <v>99000</v>
       </c>
-      <c r="F10" s="3">
+      <c r="G10" s="2">
         <v>4</v>
       </c>
-      <c r="G10" s="3">
+      <c r="H10" s="2">
         <v>2021</v>
       </c>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="3">
+      <c r="F11" s="2">
         <v>99000</v>
       </c>
-      <c r="F11" s="3">
+      <c r="G11" s="2">
         <v>11</v>
       </c>
-      <c r="G11" s="3">
+      <c r="H11" s="2">
         <v>2021</v>
       </c>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="3">
+      <c r="F12" s="2">
         <v>189000</v>
       </c>
-      <c r="F12" s="3">
+      <c r="G12" s="2">
         <v>6</v>
       </c>
-      <c r="G12" s="3">
+      <c r="H12" s="2">
         <v>2019</v>
       </c>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="3">
+      <c r="F13" s="2">
         <v>130500</v>
       </c>
-      <c r="F13" s="3">
+      <c r="G13" s="2">
         <v>11</v>
       </c>
-      <c r="G13" s="3">
+      <c r="H13" s="2">
         <v>2021</v>
       </c>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="3">
+      <c r="F14" s="2">
         <v>150000</v>
       </c>
-      <c r="F14" s="3">
+      <c r="G14" s="2">
         <v>16</v>
       </c>
-      <c r="G14" s="3">
+      <c r="H14" s="2">
         <v>2021</v>
       </c>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="3">
+      <c r="F15" s="2">
         <v>85000</v>
       </c>
-      <c r="F15" s="3">
+      <c r="G15" s="2">
         <v>11</v>
       </c>
-      <c r="G15" s="3">
+      <c r="H15" s="2">
         <v>2021</v>
       </c>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="3">
+      <c r="F16" s="2">
         <v>110000</v>
       </c>
-      <c r="F16" s="3">
+      <c r="G16" s="2">
         <v>16</v>
       </c>
-      <c r="G16" s="3">
+      <c r="H16" s="2">
         <v>2021</v>
       </c>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="3">
+      <c r="F17" s="2">
         <v>80000</v>
       </c>
-      <c r="F17" s="3">
+      <c r="G17" s="2">
         <v>11</v>
       </c>
-      <c r="G17" s="3">
+      <c r="H17" s="2">
         <v>2021</v>
       </c>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E18" s="3">
+      <c r="F18" s="2">
         <v>100000</v>
       </c>
-      <c r="F18" s="3">
+      <c r="G18" s="2">
         <v>18</v>
       </c>
-      <c r="G18" s="3">
+      <c r="H18" s="2">
         <v>2020</v>
       </c>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="3">
+      <c r="F19" s="2">
         <v>79000</v>
       </c>
-      <c r="F19" s="3">
+      <c r="G19" s="2">
         <v>26</v>
       </c>
-      <c r="G19" s="3">
+      <c r="H19" s="2">
         <v>2021</v>
       </c>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="3">
+      <c r="F20" s="2">
         <v>228000</v>
       </c>
-      <c r="F20" s="3">
+      <c r="G20" s="2">
         <v>21</v>
       </c>
-      <c r="G20" s="3">
+      <c r="H20" s="2">
         <v>2022</v>
       </c>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="E21" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="3">
+      <c r="F21" s="2">
         <v>135000</v>
       </c>
-      <c r="F21" s="3">
+      <c r="G21" s="2">
         <v>23</v>
       </c>
-      <c r="G21" s="3">
+      <c r="H21" s="2">
         <v>2017</v>
       </c>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="E22" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="3">
+      <c r="F22" s="2">
         <v>99000</v>
       </c>
-      <c r="F22" s="3">
+      <c r="G22" s="2">
         <v>15</v>
       </c>
-      <c r="G22" s="3">
+      <c r="H22" s="2">
         <v>2017</v>
       </c>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E23" s="3">
+      <c r="F23" s="2">
         <v>180000</v>
       </c>
-      <c r="F23" s="3">
+      <c r="G23" s="2">
         <v>16</v>
       </c>
-      <c r="G23" s="3">
+      <c r="H23" s="2">
         <v>2017</v>
       </c>
-      <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="E24" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E24" s="3">
+      <c r="F24" s="2">
         <v>270000</v>
       </c>
-      <c r="F24" s="3">
+      <c r="G24" s="2">
         <v>19</v>
       </c>
-      <c r="G24" s="3">
+      <c r="H24" s="2">
         <v>2017</v>
       </c>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="E25" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E25" s="3">
+      <c r="F25" s="2">
         <v>355000</v>
       </c>
-      <c r="F25" s="3">
+      <c r="G25" s="2">
         <v>17</v>
       </c>
-      <c r="G25" s="3">
+      <c r="H25" s="2">
         <v>2017</v>
       </c>
-      <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E26" s="3">
+      <c r="F26" s="2">
         <v>215000</v>
       </c>
-      <c r="F26" s="3">
+      <c r="G26" s="2">
         <v>25</v>
       </c>
-      <c r="G26" s="3">
+      <c r="H26" s="2">
         <v>2017</v>
       </c>
-      <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="E27" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E27" s="3">
+      <c r="F27" s="2">
         <v>245000</v>
       </c>
-      <c r="F27" s="3">
+      <c r="G27" s="2">
         <v>15</v>
       </c>
-      <c r="G27" s="3">
+      <c r="H27" s="2">
         <v>2017</v>
       </c>
-      <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="E28" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E28" s="3">
+      <c r="F28" s="2">
         <v>108000</v>
       </c>
-      <c r="F28" s="3">
+      <c r="G28" s="2">
         <v>17</v>
       </c>
-      <c r="G28" s="3">
+      <c r="H28" s="2">
         <v>2018</v>
       </c>
-      <c r="J28" s="1"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="E29" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E29" s="3">
+      <c r="F29" s="2">
         <v>96000</v>
       </c>
-      <c r="F29" s="3">
+      <c r="G29" s="2">
         <v>20</v>
       </c>
-      <c r="G29" s="3">
+      <c r="H29" s="2">
         <v>2022</v>
       </c>
-      <c r="J29" s="1"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="E30" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E30" s="3">
+      <c r="F30" s="2">
         <v>60000</v>
       </c>
-      <c r="F30" s="3">
+      <c r="G30" s="2">
         <v>14</v>
       </c>
-      <c r="G30" s="3">
+      <c r="H30" s="2">
         <v>2016</v>
       </c>
-      <c r="J30" s="1"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="E31" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E31" s="3">
+      <c r="F31" s="2">
         <v>163250</v>
       </c>
-      <c r="F31" s="3">
+      <c r="G31" s="2">
         <v>22</v>
       </c>
-      <c r="G31" s="3">
+      <c r="H31" s="2">
         <v>2021</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B32" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="E32" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E32" s="3">
+      <c r="F32" s="2">
         <v>149000</v>
       </c>
-      <c r="F32" s="3">
+      <c r="G32" s="2">
         <v>16</v>
       </c>
-      <c r="G32" s="3">
+      <c r="H32" s="2">
         <v>2021</v>
       </c>
     </row>

</xml_diff>